<commit_message>
ATL 2023 initial template
</commit_message>
<xml_diff>
--- a/assets/misc/2022/2022_Attendance.xlsx
+++ b/assets/misc/2022/2022_Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F199A90-AB78-4912-9D93-F116AF67648C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B610117-6A24-49BE-ABA2-95B05D9F74CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="570" windowWidth="13830" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -124,10 +132,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +421,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,19 +433,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -454,67 +463,64 @@
         <v>252</v>
       </c>
       <c r="E2" s="2">
-        <f>+(C2-D2)/C2</f>
+        <f t="shared" ref="E2:E18" si="0">+(C2-D2)/C2</f>
         <v>0.37931034482758619</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>44856</v>
-      </c>
-      <c r="D3">
-        <v>115</v>
+        <v>44769</v>
       </c>
       <c r="E3" s="2" t="e">
-        <f t="shared" ref="E3:E18" si="0">+(C3-D3)/C3</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>44856</v>
+        <v>44779</v>
       </c>
       <c r="C4">
-        <v>115</v>
+        <v>483</v>
       </c>
       <c r="D4">
-        <v>60</v>
+        <v>183</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0.47826086956521741</v>
+        <v>0.6211180124223602</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>44849</v>
+        <v>44786</v>
       </c>
       <c r="C5">
-        <v>75</v>
+        <v>209</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.50239234449760761</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>44786</v>
+        <v>44821</v>
       </c>
       <c r="E6" s="2" t="e">
         <f t="shared" si="0"/>
@@ -532,11 +538,11 @@
         <v>283</v>
       </c>
       <c r="D7">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0.4628975265017668</v>
+        <v>0.49823321554770317</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,32 +552,44 @@
       <c r="B8" s="1">
         <v>44842</v>
       </c>
-      <c r="E8" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="C8">
+        <v>240</v>
+      </c>
+      <c r="D8">
+        <v>110</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>44821</v>
-      </c>
-      <c r="E9" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>44849</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>44779</v>
+        <v>44856</v>
       </c>
       <c r="D10">
-        <v>187</v>
+        <v>115</v>
       </c>
       <c r="E10" s="2" t="e">
         <f t="shared" si="0"/>
@@ -580,59 +598,48 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
-        <v>44769</v>
-      </c>
-      <c r="E11" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>44856</v>
+      </c>
+      <c r="C11">
+        <v>115</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47826086956521741</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
+    <sortCondition ref="B2:B18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>